<commit_message>
draw hp bar for unit
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Job.xlsx
+++ b/ConfigData/Xlsx/Job.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="116">
   <si>
     <t>arrow</t>
   </si>
@@ -221,7 +221,127 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>JobIndex</t>
+    <t>颜色</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Color</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yellow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pink</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brown</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Purple</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Green</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死灵</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkfire</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gray</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在所有的黑魔法中最为黑暗的毫无疑问的非死灵术/通幽术（Necromancy）莫属！而且也是最丑恶和最令人厌恶的魔法仪式之一。而死灵术本身是指古代与死亡世界沟通的一种方法。死灵魔法可以追述到古波斯、希腊、罗马和中世纪的巫师。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>猎人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Salmon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blue</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>萨满</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aqua</t>
+  </si>
+  <si>
+    <t>electball</t>
+  </si>
+  <si>
+    <t>萨满祭司是自己部落和氏族的精神领袖。他们是操纵元素的大师，既能引导能量摧毁敌人，也能汇聚法力增强队友。在各种图腾的帮助下，萨满能凝聚不羁元素的能量，化身为全能的战士。</t>
+  </si>
+  <si>
+    <t>萨满</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷系</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>法术</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动2</t>
+  </si>
+  <si>
+    <t>坟墓</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否特殊职业</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>野怪</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -229,11 +349,19 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>颜色</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Color</t>
+    <t>SkillId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsSpecial</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>别名</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -241,142 +369,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Yellow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pink</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brown</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Purple</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Green</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死灵</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>darkfire</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gray</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>在所有的黑魔法中最为黑暗的毫无疑问的非死灵术/通幽术（Necromancy）莫属！而且也是最丑恶和最令人厌恶的魔法仪式之一。而死灵术本身是指古代与死亡世界沟通的一种方法。死灵魔法可以追述到古波斯、希腊、罗马和中世纪的巫师。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>猎人</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Salmon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Blue</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>萨满</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Aqua</t>
-  </si>
-  <si>
-    <t>electball</t>
-  </si>
-  <si>
-    <t>萨满祭司是自己部落和氏族的精神领袖。他们是操纵元素的大师，既能引导能量摧毁敌人，也能汇聚法力增强队友。在各种图腾的帮助下，萨满能凝聚不羁元素的能量，化身为全能的战士。</t>
-  </si>
-  <si>
-    <t>萨满</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>雷系</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>法术</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>活动1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>活动2</t>
-  </si>
-  <si>
-    <t>坟墓</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否特殊职业</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>野怪</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>技能</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>IsSpecial</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string[]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>别名</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Alias</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -433,6 +425,14 @@
   </si>
   <si>
     <t>Mag</t>
+  </si>
+  <si>
+    <t>Icon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jian</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1190,35 +1190,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1329,6 +1300,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1834,13 +1834,13 @@
     <tableColumn id="10" name="Skl" dataDxfId="9"/>
     <tableColumn id="14" name="Luk" dataDxfId="8"/>
     <tableColumn id="16" name="Mov" dataDxfId="7"/>
-    <tableColumn id="20" name="Mag" dataDxfId="0"/>
-    <tableColumn id="17" name="Hp" dataDxfId="6"/>
-    <tableColumn id="7" name="SkillId" dataDxfId="5"/>
-    <tableColumn id="9" name="InitialItem" dataDxfId="4"/>
-    <tableColumn id="11" name="JobIndex" dataDxfId="3"/>
-    <tableColumn id="12" name="Color" dataDxfId="2"/>
-    <tableColumn id="13" name="IsSpecial" dataDxfId="1"/>
+    <tableColumn id="20" name="Mag" dataDxfId="6"/>
+    <tableColumn id="17" name="Hp" dataDxfId="5"/>
+    <tableColumn id="7" name="SkillId" dataDxfId="4"/>
+    <tableColumn id="9" name="InitialItem" dataDxfId="3"/>
+    <tableColumn id="11" name="Icon" dataDxfId="2"/>
+    <tableColumn id="12" name="Color" dataDxfId="1"/>
+    <tableColumn id="13" name="IsSpecial" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2170,7 +2170,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2191,7 +2191,7 @@
         <v>19</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>20</v>
@@ -2203,31 +2203,31 @@
         <v>22</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>112</v>
-      </c>
       <c r="N1" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O1" s="8" t="s">
         <v>34</v>
@@ -2236,10 +2236,10 @@
         <v>29</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
@@ -2247,7 +2247,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>18</v>
@@ -2259,43 +2259,43 @@
         <v>18</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.15">
@@ -2303,7 +2303,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>14</v>
@@ -2315,43 +2315,43 @@
         <v>16</v>
       </c>
       <c r="F3" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="L3" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M3" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="K3" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="N3" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>33</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R3" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
@@ -2359,7 +2359,7 @@
         <v>11000000</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>23</v>
@@ -2392,14 +2392,14 @@
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="2">
-        <v>0</v>
+      <c r="P4" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.15">
@@ -2442,11 +2442,11 @@
         <v>31000001</v>
       </c>
       <c r="O5" s="11"/>
-      <c r="P5" s="2">
-        <v>1</v>
+      <c r="P5" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R5" s="11"/>
     </row>
@@ -2490,11 +2490,11 @@
         <v>31000002</v>
       </c>
       <c r="O6" s="11"/>
-      <c r="P6" s="2">
-        <v>2</v>
+      <c r="P6" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R6" s="11"/>
     </row>
@@ -2538,11 +2538,11 @@
         <v>31000003</v>
       </c>
       <c r="O7" s="11"/>
-      <c r="P7" s="2">
-        <v>3</v>
+      <c r="P7" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R7" s="11"/>
     </row>
@@ -2552,7 +2552,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>0</v>
@@ -2586,11 +2586,11 @@
         <v>31000004</v>
       </c>
       <c r="O8" s="11"/>
-      <c r="P8" s="2">
-        <v>4</v>
+      <c r="P8" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R8" s="11"/>
     </row>
@@ -2634,11 +2634,11 @@
         <v>31000005</v>
       </c>
       <c r="O9" s="11"/>
-      <c r="P9" s="2">
-        <v>5</v>
+      <c r="P9" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R9" s="11"/>
     </row>
@@ -2682,11 +2682,11 @@
         <v>31000006</v>
       </c>
       <c r="O10" s="11"/>
-      <c r="P10" s="2">
-        <v>6</v>
+      <c r="P10" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="R10" s="11"/>
     </row>
@@ -2730,11 +2730,11 @@
         <v>31000007</v>
       </c>
       <c r="O11" s="11"/>
-      <c r="P11" s="2">
-        <v>7</v>
+      <c r="P11" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R11" s="11"/>
     </row>
@@ -2778,11 +2778,11 @@
         <v>31000008</v>
       </c>
       <c r="O12" s="11"/>
-      <c r="P12" s="2">
-        <v>8</v>
+      <c r="P12" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R12" s="11"/>
     </row>
@@ -2792,13 +2792,13 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="F13" s="2">
         <v>5</v>
@@ -2826,11 +2826,11 @@
         <v>31000009</v>
       </c>
       <c r="O13" s="11"/>
-      <c r="P13" s="2">
-        <v>9</v>
+      <c r="P13" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="R13" s="11"/>
     </row>
@@ -2840,13 +2840,13 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F14" s="2">
         <v>5</v>
@@ -2874,11 +2874,11 @@
         <v>31000010</v>
       </c>
       <c r="O14" s="11"/>
-      <c r="P14" s="2">
-        <v>10</v>
+      <c r="P14" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R14" s="11"/>
     </row>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>2</v>
@@ -2904,14 +2904,14 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="11"/>
-      <c r="P15" s="2">
-        <v>0</v>
+      <c r="P15" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.15">
@@ -2920,7 +2920,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>2</v>
@@ -2936,14 +2936,14 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="11"/>
-      <c r="P16" s="2">
-        <v>0</v>
+      <c r="P16" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.15">
@@ -2952,7 +2952,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>2</v>
@@ -2968,14 +2968,14 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="11"/>
-      <c r="P17" s="2">
-        <v>0</v>
+      <c r="P17" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3104,7 +3104,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G9" t="s">
         <v>51</v>
@@ -3123,21 +3123,21 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>